<commit_message>
Add Swab & Sputum & Stool E gene Ct value
</commit_message>
<xml_diff>
--- a/data/kim2020viral/kim2020viral.xlsx
+++ b/data/kim2020viral/kim2020viral.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fionaxiao/Desktop/shedding-hub/data/kim2020viral/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC41A98-4959-1641-ADC6-15B9E8AA4872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2A7485-E93E-264F-AC05-C8F5BC235C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1200" yWindow="760" windowWidth="27240" windowHeight="16240" xr2:uid="{4A3A77D9-3CB4-3B4A-85E5-EADE8C06CB15}"/>
   </bookViews>
@@ -65,25 +65,25 @@
     <t>Value</t>
   </si>
   <si>
-    <t>swab RdRp estimated viral copy/mL</t>
-  </si>
-  <si>
     <t>ud</t>
   </si>
   <si>
-    <t>sputum RdRp estimated viral copy/mL</t>
+    <t>swab_SARSCoV2_E_Ct</t>
   </si>
   <si>
-    <t>swab E</t>
+    <t>sputum_SARSCoV2_E_Ct</t>
   </si>
   <si>
-    <t>sputum E</t>
+    <t>stool_SARSCoV2_RdRp_Ct</t>
   </si>
   <si>
-    <t>stool RdRp</t>
+    <t>stool_SARSCoV2_E_Ct</t>
   </si>
   <si>
-    <t>stool E</t>
+    <t>sputum_SARSCoV2_RdRp_VL</t>
+  </si>
+  <si>
+    <t>swab_SARSCoV2_RdRp_VL</t>
   </si>
 </sst>
 </file>
@@ -457,8 +457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AA1B1AD-FEF0-AB4A-965C-49BDF551413D}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="M89" sqref="M89"/>
+    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -506,7 +506,7 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -529,7 +529,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -552,7 +552,7 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -575,7 +575,7 @@
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -598,7 +598,7 @@
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -621,7 +621,7 @@
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -644,7 +644,7 @@
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -667,7 +667,7 @@
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -690,7 +690,7 @@
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -713,7 +713,7 @@
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -730,13 +730,13 @@
         <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -759,7 +759,7 @@
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -776,13 +776,13 @@
         <v>5</v>
       </c>
       <c r="E14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F14">
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -799,13 +799,13 @@
         <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F15">
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -828,7 +828,7 @@
         <v>2</v>
       </c>
       <c r="G16" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -851,7 +851,7 @@
         <v>2</v>
       </c>
       <c r="G17" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -868,13 +868,13 @@
         <v>6</v>
       </c>
       <c r="E18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F18">
         <v>2</v>
       </c>
       <c r="G18" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -897,7 +897,7 @@
         <v>2</v>
       </c>
       <c r="G19" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -914,13 +914,13 @@
         <v>6</v>
       </c>
       <c r="E20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20">
         <v>2</v>
       </c>
       <c r="G20" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -937,13 +937,13 @@
         <v>6</v>
       </c>
       <c r="E21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F21">
         <v>2</v>
       </c>
       <c r="G21" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -960,13 +960,13 @@
         <v>6</v>
       </c>
       <c r="E22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F22">
         <v>2</v>
       </c>
       <c r="G22" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -983,13 +983,13 @@
         <v>6</v>
       </c>
       <c r="E23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F23">
         <v>2</v>
       </c>
       <c r="G23" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1006,13 +1006,13 @@
         <v>6</v>
       </c>
       <c r="E24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F24">
         <v>2</v>
       </c>
       <c r="G24" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -1029,13 +1029,13 @@
         <v>6</v>
       </c>
       <c r="E25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F25">
         <v>2</v>
       </c>
       <c r="G25" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -1058,7 +1058,7 @@
         <v>2</v>
       </c>
       <c r="G26" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -1075,13 +1075,13 @@
         <v>6</v>
       </c>
       <c r="E27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F27">
         <v>2</v>
       </c>
       <c r="G27" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1104,7 +1104,7 @@
         <v>1</v>
       </c>
       <c r="G28" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1127,7 +1127,7 @@
         <v>1</v>
       </c>
       <c r="G29" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -1150,7 +1150,7 @@
         <v>1</v>
       </c>
       <c r="G30" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -1173,7 +1173,7 @@
         <v>1</v>
       </c>
       <c r="G31" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -1196,7 +1196,7 @@
         <v>1</v>
       </c>
       <c r="G32" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -1213,13 +1213,13 @@
         <v>5</v>
       </c>
       <c r="E33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F33">
         <v>1</v>
       </c>
       <c r="G33" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -1242,7 +1242,7 @@
         <v>1</v>
       </c>
       <c r="G34" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -1265,7 +1265,7 @@
         <v>1</v>
       </c>
       <c r="G35" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -1288,7 +1288,7 @@
         <v>1</v>
       </c>
       <c r="G36" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -1311,7 +1311,7 @@
         <v>1</v>
       </c>
       <c r="G37" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -1328,13 +1328,13 @@
         <v>5</v>
       </c>
       <c r="E38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F38">
         <v>1</v>
       </c>
       <c r="G38" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -1351,13 +1351,13 @@
         <v>5</v>
       </c>
       <c r="E39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F39">
         <v>1</v>
       </c>
       <c r="G39" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
@@ -1374,13 +1374,13 @@
         <v>5</v>
       </c>
       <c r="E40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F40">
         <v>1</v>
       </c>
       <c r="G40" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -1403,7 +1403,7 @@
         <v>2</v>
       </c>
       <c r="G41" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -1420,13 +1420,13 @@
         <v>6</v>
       </c>
       <c r="E42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F42">
         <v>2</v>
       </c>
       <c r="G42" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -1443,13 +1443,13 @@
         <v>6</v>
       </c>
       <c r="E43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F43">
         <v>2</v>
       </c>
       <c r="G43" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -1466,13 +1466,13 @@
         <v>6</v>
       </c>
       <c r="E44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F44">
         <v>2</v>
       </c>
       <c r="G44" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -1489,13 +1489,13 @@
         <v>6</v>
       </c>
       <c r="E45" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F45">
         <v>2</v>
       </c>
       <c r="G45" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
@@ -1512,13 +1512,13 @@
         <v>6</v>
       </c>
       <c r="E46" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F46">
         <v>2</v>
       </c>
       <c r="G46" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -1535,13 +1535,13 @@
         <v>6</v>
       </c>
       <c r="E47" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F47">
         <v>2</v>
       </c>
       <c r="G47" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
@@ -1561,7 +1561,7 @@
         <v>1</v>
       </c>
       <c r="G48" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
@@ -1581,7 +1581,7 @@
         <v>1</v>
       </c>
       <c r="G49" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
@@ -1601,7 +1601,7 @@
         <v>1</v>
       </c>
       <c r="G50" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -1621,7 +1621,7 @@
         <v>1</v>
       </c>
       <c r="G51" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
@@ -1641,7 +1641,7 @@
         <v>1</v>
       </c>
       <c r="G52" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
@@ -1661,7 +1661,7 @@
         <v>1</v>
       </c>
       <c r="G53" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
@@ -1675,13 +1675,13 @@
         <v>5</v>
       </c>
       <c r="E54" t="s">
+        <v>9</v>
+      </c>
+      <c r="F54">
+        <v>1</v>
+      </c>
+      <c r="G54" t="s">
         <v>10</v>
-      </c>
-      <c r="F54">
-        <v>1</v>
-      </c>
-      <c r="G54" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
@@ -1695,13 +1695,13 @@
         <v>5</v>
       </c>
       <c r="E55" t="s">
+        <v>9</v>
+      </c>
+      <c r="F55">
+        <v>1</v>
+      </c>
+      <c r="G55" t="s">
         <v>10</v>
-      </c>
-      <c r="F55">
-        <v>1</v>
-      </c>
-      <c r="G55" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
@@ -1721,7 +1721,7 @@
         <v>1</v>
       </c>
       <c r="G56" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
@@ -1741,7 +1741,7 @@
         <v>1</v>
       </c>
       <c r="G57" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
@@ -1755,13 +1755,13 @@
         <v>5</v>
       </c>
       <c r="E58" t="s">
+        <v>9</v>
+      </c>
+      <c r="F58">
+        <v>1</v>
+      </c>
+      <c r="G58" t="s">
         <v>10</v>
-      </c>
-      <c r="F58">
-        <v>1</v>
-      </c>
-      <c r="G58" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
@@ -1781,7 +1781,7 @@
         <v>1</v>
       </c>
       <c r="G59" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
@@ -1795,13 +1795,13 @@
         <v>5</v>
       </c>
       <c r="E60" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60">
+        <v>1</v>
+      </c>
+      <c r="G60" t="s">
         <v>10</v>
-      </c>
-      <c r="F60">
-        <v>1</v>
-      </c>
-      <c r="G60" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
@@ -1815,13 +1815,13 @@
         <v>5</v>
       </c>
       <c r="E61" t="s">
+        <v>9</v>
+      </c>
+      <c r="F61">
+        <v>1</v>
+      </c>
+      <c r="G61" t="s">
         <v>10</v>
-      </c>
-      <c r="F61">
-        <v>1</v>
-      </c>
-      <c r="G61" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
@@ -1841,7 +1841,7 @@
         <v>2</v>
       </c>
       <c r="G62" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
@@ -1861,7 +1861,7 @@
         <v>2</v>
       </c>
       <c r="G63" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
@@ -1881,7 +1881,7 @@
         <v>2</v>
       </c>
       <c r="G64" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
@@ -1901,7 +1901,7 @@
         <v>2</v>
       </c>
       <c r="G65" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
@@ -1915,13 +1915,13 @@
         <v>6</v>
       </c>
       <c r="E66" t="s">
+        <v>9</v>
+      </c>
+      <c r="F66">
+        <v>2</v>
+      </c>
+      <c r="G66" t="s">
         <v>10</v>
-      </c>
-      <c r="F66">
-        <v>2</v>
-      </c>
-      <c r="G66" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
@@ -1935,13 +1935,13 @@
         <v>6</v>
       </c>
       <c r="E67" t="s">
+        <v>9</v>
+      </c>
+      <c r="F67">
+        <v>2</v>
+      </c>
+      <c r="G67" t="s">
         <v>10</v>
-      </c>
-      <c r="F67">
-        <v>2</v>
-      </c>
-      <c r="G67" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
@@ -1955,13 +1955,13 @@
         <v>6</v>
       </c>
       <c r="E68" t="s">
+        <v>9</v>
+      </c>
+      <c r="F68">
+        <v>2</v>
+      </c>
+      <c r="G68" t="s">
         <v>10</v>
-      </c>
-      <c r="F68">
-        <v>2</v>
-      </c>
-      <c r="G68" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
@@ -1975,13 +1975,13 @@
         <v>6</v>
       </c>
       <c r="E69" t="s">
+        <v>9</v>
+      </c>
+      <c r="F69">
+        <v>2</v>
+      </c>
+      <c r="G69" t="s">
         <v>10</v>
-      </c>
-      <c r="F69">
-        <v>2</v>
-      </c>
-      <c r="G69" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
@@ -1995,13 +1995,13 @@
         <v>6</v>
       </c>
       <c r="E70" t="s">
+        <v>9</v>
+      </c>
+      <c r="F70">
+        <v>2</v>
+      </c>
+      <c r="G70" t="s">
         <v>10</v>
-      </c>
-      <c r="F70">
-        <v>2</v>
-      </c>
-      <c r="G70" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
@@ -2015,13 +2015,13 @@
         <v>6</v>
       </c>
       <c r="E71" t="s">
+        <v>9</v>
+      </c>
+      <c r="F71">
+        <v>2</v>
+      </c>
+      <c r="G71" t="s">
         <v>10</v>
-      </c>
-      <c r="F71">
-        <v>2</v>
-      </c>
-      <c r="G71" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
@@ -2041,7 +2041,7 @@
         <v>2</v>
       </c>
       <c r="G72" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
@@ -2055,13 +2055,13 @@
         <v>6</v>
       </c>
       <c r="E73" t="s">
+        <v>9</v>
+      </c>
+      <c r="F73">
+        <v>2</v>
+      </c>
+      <c r="G73" t="s">
         <v>10</v>
-      </c>
-      <c r="F73">
-        <v>2</v>
-      </c>
-      <c r="G73" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
@@ -2081,7 +2081,7 @@
         <v>1</v>
       </c>
       <c r="G74" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
@@ -2101,7 +2101,7 @@
         <v>1</v>
       </c>
       <c r="G75" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
@@ -2121,7 +2121,7 @@
         <v>1</v>
       </c>
       <c r="G76" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
@@ -2141,7 +2141,7 @@
         <v>1</v>
       </c>
       <c r="G77" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
@@ -2161,7 +2161,7 @@
         <v>1</v>
       </c>
       <c r="G78" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
@@ -2175,13 +2175,13 @@
         <v>5</v>
       </c>
       <c r="E79" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F79">
         <v>1</v>
       </c>
       <c r="G79" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
@@ -2195,13 +2195,13 @@
         <v>5</v>
       </c>
       <c r="E80" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F80">
         <v>1</v>
       </c>
       <c r="G80" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
@@ -2221,7 +2221,7 @@
         <v>1</v>
       </c>
       <c r="G81" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
@@ -2235,13 +2235,13 @@
         <v>5</v>
       </c>
       <c r="E82" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F82">
         <v>1</v>
       </c>
       <c r="G82" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
@@ -2255,13 +2255,13 @@
         <v>5</v>
       </c>
       <c r="E83" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F83">
         <v>1</v>
       </c>
       <c r="G83" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
@@ -2275,13 +2275,13 @@
         <v>5</v>
       </c>
       <c r="E84" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F84">
         <v>1</v>
       </c>
       <c r="G84" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
@@ -2295,13 +2295,13 @@
         <v>5</v>
       </c>
       <c r="E85" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F85">
         <v>1</v>
       </c>
       <c r="G85" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
@@ -2315,13 +2315,13 @@
         <v>5</v>
       </c>
       <c r="E86" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F86">
         <v>1</v>
       </c>
       <c r="G86" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
@@ -2341,7 +2341,7 @@
         <v>2</v>
       </c>
       <c r="G87" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
@@ -2355,13 +2355,13 @@
         <v>6</v>
       </c>
       <c r="E88" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F88">
         <v>2</v>
       </c>
       <c r="G88" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
@@ -2375,13 +2375,13 @@
         <v>6</v>
       </c>
       <c r="E89" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F89">
         <v>2</v>
       </c>
       <c r="G89" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
@@ -2395,13 +2395,13 @@
         <v>6</v>
       </c>
       <c r="E90" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F90">
         <v>2</v>
       </c>
       <c r="G90" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
@@ -2415,13 +2415,13 @@
         <v>6</v>
       </c>
       <c r="E91" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F91">
         <v>2</v>
       </c>
       <c r="G91" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
@@ -2435,13 +2435,13 @@
         <v>6</v>
       </c>
       <c r="E92" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F92">
         <v>2</v>
       </c>
       <c r="G92" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
@@ -2461,7 +2461,7 @@
         <v>2</v>
       </c>
       <c r="G93" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
@@ -2475,13 +2475,13 @@
         <v>5</v>
       </c>
       <c r="E94" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F94">
         <v>1</v>
       </c>
       <c r="G94" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
@@ -2495,13 +2495,13 @@
         <v>5</v>
       </c>
       <c r="E95" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F95">
         <v>1</v>
       </c>
       <c r="G95" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
@@ -2515,13 +2515,13 @@
         <v>5</v>
       </c>
       <c r="E96" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F96">
         <v>1</v>
       </c>
       <c r="G96" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
@@ -2541,7 +2541,7 @@
         <v>1</v>
       </c>
       <c r="G97" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
@@ -2555,13 +2555,13 @@
         <v>5</v>
       </c>
       <c r="E98" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F98">
         <v>1</v>
       </c>
       <c r="G98" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
@@ -2575,13 +2575,13 @@
         <v>5</v>
       </c>
       <c r="E99" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F99">
         <v>1</v>
       </c>
       <c r="G99" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
@@ -2601,7 +2601,7 @@
         <v>1</v>
       </c>
       <c r="G100" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
@@ -2621,7 +2621,7 @@
         <v>1</v>
       </c>
       <c r="G101" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
@@ -2635,13 +2635,13 @@
         <v>5</v>
       </c>
       <c r="E102" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F102">
         <v>1</v>
       </c>
       <c r="G102" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
@@ -2655,13 +2655,13 @@
         <v>5</v>
       </c>
       <c r="E103" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F103">
         <v>1</v>
       </c>
       <c r="G103" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
@@ -2675,13 +2675,13 @@
         <v>5</v>
       </c>
       <c r="E104" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F104">
         <v>1</v>
       </c>
       <c r="G104" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
@@ -2701,7 +2701,7 @@
         <v>1</v>
       </c>
       <c r="G105" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
@@ -2721,7 +2721,7 @@
         <v>1</v>
       </c>
       <c r="G106" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
@@ -2741,7 +2741,7 @@
         <v>1</v>
       </c>
       <c r="G107" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
@@ -2761,7 +2761,7 @@
         <v>1</v>
       </c>
       <c r="G108" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
@@ -2775,13 +2775,13 @@
         <v>5</v>
       </c>
       <c r="E109" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F109">
         <v>1</v>
       </c>
       <c r="G109" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
@@ -2801,7 +2801,7 @@
         <v>1</v>
       </c>
       <c r="G110" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
@@ -2815,13 +2815,13 @@
         <v>5</v>
       </c>
       <c r="E111" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F111">
         <v>1</v>
       </c>
       <c r="G111" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
@@ -2835,13 +2835,13 @@
         <v>5</v>
       </c>
       <c r="E112" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F112">
         <v>1</v>
       </c>
       <c r="G112" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
@@ -2855,13 +2855,13 @@
         <v>5</v>
       </c>
       <c r="E113" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F113">
         <v>1</v>
       </c>
       <c r="G113" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.2">
@@ -2875,13 +2875,13 @@
         <v>5</v>
       </c>
       <c r="E114" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F114">
         <v>1</v>
       </c>
       <c r="G114" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
@@ -2895,13 +2895,13 @@
         <v>5</v>
       </c>
       <c r="E115" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F115">
         <v>1</v>
       </c>
       <c r="G115" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
@@ -2915,13 +2915,13 @@
         <v>6</v>
       </c>
       <c r="E116" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F116">
         <v>2</v>
       </c>
       <c r="G116" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
@@ -2935,13 +2935,13 @@
         <v>6</v>
       </c>
       <c r="E117" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F117">
         <v>2</v>
       </c>
       <c r="G117" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
@@ -2955,13 +2955,13 @@
         <v>6</v>
       </c>
       <c r="E118" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F118">
         <v>2</v>
       </c>
       <c r="G118" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
@@ -2975,13 +2975,13 @@
         <v>6</v>
       </c>
       <c r="E119" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F119">
         <v>2</v>
       </c>
       <c r="G119" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.2">
@@ -2995,13 +2995,13 @@
         <v>6</v>
       </c>
       <c r="E120" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F120">
         <v>2</v>
       </c>
       <c r="G120" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.2">
@@ -3015,13 +3015,13 @@
         <v>6</v>
       </c>
       <c r="E121" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F121">
         <v>2</v>
       </c>
       <c r="G121" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.2">
@@ -3041,7 +3041,7 @@
         <v>2</v>
       </c>
       <c r="G122" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.2">
@@ -3055,13 +3055,13 @@
         <v>6</v>
       </c>
       <c r="E123" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F123">
         <v>2</v>
       </c>
       <c r="G123" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.2">
@@ -3075,13 +3075,13 @@
         <v>6</v>
       </c>
       <c r="E124" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F124">
         <v>2</v>
       </c>
       <c r="G124" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.2">
@@ -3095,13 +3095,13 @@
         <v>6</v>
       </c>
       <c r="E125" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F125">
         <v>2</v>
       </c>
       <c r="G125" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add sputum_SARSCoV2_RdRp_Ct and swab_SARSCoV2_RdRp_Ct
</commit_message>
<xml_diff>
--- a/data/kim2020viral/kim2020viral.xlsx
+++ b/data/kim2020viral/kim2020viral.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fionaxiao/Desktop/shedding-hub/data/kim2020viral/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2A7485-E93E-264F-AC05-C8F5BC235C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB48490-765E-D343-881D-50C6DD53A6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1200" yWindow="760" windowWidth="27240" windowHeight="16240" xr2:uid="{4A3A77D9-3CB4-3B4A-85E5-EADE8C06CB15}"/>
   </bookViews>
@@ -68,22 +68,22 @@
     <t>ud</t>
   </si>
   <si>
-    <t>swab_SARSCoV2_E_Ct</t>
+    <t>swab_SARSCoV2_RdRp</t>
   </si>
   <si>
-    <t>sputum_SARSCoV2_E_Ct</t>
+    <t>sputum_SARSCoV2_RdRp</t>
   </si>
   <si>
-    <t>stool_SARSCoV2_RdRp_Ct</t>
+    <t>swab_SARSCoV2_E</t>
   </si>
   <si>
-    <t>stool_SARSCoV2_E_Ct</t>
+    <t>sputum_SARSCoV2_E</t>
   </si>
   <si>
-    <t>sputum_SARSCoV2_RdRp_VL</t>
+    <t>stool_SARSCoV2_RdRp</t>
   </si>
   <si>
-    <t>swab_SARSCoV2_RdRp_VL</t>
+    <t>stool_SARSCoV2_E</t>
   </si>
 </sst>
 </file>
@@ -457,8 +457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AA1B1AD-FEF0-AB4A-965C-49BDF551413D}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A105" zoomScale="140" workbookViewId="0">
+      <selection activeCell="G127" sqref="G127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -506,7 +506,7 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -529,7 +529,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -552,7 +552,7 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -575,7 +575,7 @@
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -598,7 +598,7 @@
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -621,7 +621,7 @@
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -644,7 +644,7 @@
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -667,7 +667,7 @@
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -690,7 +690,7 @@
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -713,7 +713,7 @@
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -736,7 +736,7 @@
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -759,7 +759,7 @@
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -782,7 +782,7 @@
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -805,7 +805,7 @@
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -828,7 +828,7 @@
         <v>2</v>
       </c>
       <c r="G16" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -851,7 +851,7 @@
         <v>2</v>
       </c>
       <c r="G17" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -874,7 +874,7 @@
         <v>2</v>
       </c>
       <c r="G18" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -897,7 +897,7 @@
         <v>2</v>
       </c>
       <c r="G19" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -920,7 +920,7 @@
         <v>2</v>
       </c>
       <c r="G20" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -943,7 +943,7 @@
         <v>2</v>
       </c>
       <c r="G21" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -966,7 +966,7 @@
         <v>2</v>
       </c>
       <c r="G22" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -989,7 +989,7 @@
         <v>2</v>
       </c>
       <c r="G23" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1012,7 +1012,7 @@
         <v>2</v>
       </c>
       <c r="G24" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -1035,7 +1035,7 @@
         <v>2</v>
       </c>
       <c r="G25" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -1058,7 +1058,7 @@
         <v>2</v>
       </c>
       <c r="G26" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -1081,7 +1081,7 @@
         <v>2</v>
       </c>
       <c r="G27" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1104,7 +1104,7 @@
         <v>1</v>
       </c>
       <c r="G28" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1127,7 +1127,7 @@
         <v>1</v>
       </c>
       <c r="G29" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -1150,7 +1150,7 @@
         <v>1</v>
       </c>
       <c r="G30" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -1173,7 +1173,7 @@
         <v>1</v>
       </c>
       <c r="G31" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -1196,7 +1196,7 @@
         <v>1</v>
       </c>
       <c r="G32" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -1219,7 +1219,7 @@
         <v>1</v>
       </c>
       <c r="G33" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -1242,7 +1242,7 @@
         <v>1</v>
       </c>
       <c r="G34" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -1265,7 +1265,7 @@
         <v>1</v>
       </c>
       <c r="G35" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -1288,7 +1288,7 @@
         <v>1</v>
       </c>
       <c r="G36" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -1311,7 +1311,7 @@
         <v>1</v>
       </c>
       <c r="G37" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -1334,7 +1334,7 @@
         <v>1</v>
       </c>
       <c r="G38" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -1357,7 +1357,7 @@
         <v>1</v>
       </c>
       <c r="G39" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
@@ -1380,7 +1380,7 @@
         <v>1</v>
       </c>
       <c r="G40" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -1403,7 +1403,7 @@
         <v>2</v>
       </c>
       <c r="G41" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -1426,7 +1426,7 @@
         <v>2</v>
       </c>
       <c r="G42" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -1449,7 +1449,7 @@
         <v>2</v>
       </c>
       <c r="G43" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -1472,7 +1472,7 @@
         <v>2</v>
       </c>
       <c r="G44" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -1495,7 +1495,7 @@
         <v>2</v>
       </c>
       <c r="G45" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
@@ -1518,7 +1518,7 @@
         <v>2</v>
       </c>
       <c r="G46" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -1541,7 +1541,7 @@
         <v>2</v>
       </c>
       <c r="G47" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
@@ -1561,7 +1561,7 @@
         <v>1</v>
       </c>
       <c r="G48" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
@@ -1581,7 +1581,7 @@
         <v>1</v>
       </c>
       <c r="G49" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
@@ -1601,7 +1601,7 @@
         <v>1</v>
       </c>
       <c r="G50" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -1621,7 +1621,7 @@
         <v>1</v>
       </c>
       <c r="G51" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
@@ -1641,7 +1641,7 @@
         <v>1</v>
       </c>
       <c r="G52" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
@@ -1661,7 +1661,7 @@
         <v>1</v>
       </c>
       <c r="G53" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
@@ -1681,7 +1681,7 @@
         <v>1</v>
       </c>
       <c r="G54" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
@@ -1701,7 +1701,7 @@
         <v>1</v>
       </c>
       <c r="G55" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
@@ -1721,7 +1721,7 @@
         <v>1</v>
       </c>
       <c r="G56" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
@@ -1741,7 +1741,7 @@
         <v>1</v>
       </c>
       <c r="G57" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
@@ -1761,7 +1761,7 @@
         <v>1</v>
       </c>
       <c r="G58" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
@@ -1781,7 +1781,7 @@
         <v>1</v>
       </c>
       <c r="G59" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
@@ -1801,7 +1801,7 @@
         <v>1</v>
       </c>
       <c r="G60" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
@@ -1821,7 +1821,7 @@
         <v>1</v>
       </c>
       <c r="G61" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
@@ -1841,7 +1841,7 @@
         <v>2</v>
       </c>
       <c r="G62" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
@@ -1861,7 +1861,7 @@
         <v>2</v>
       </c>
       <c r="G63" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
@@ -1881,7 +1881,7 @@
         <v>2</v>
       </c>
       <c r="G64" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
@@ -1901,7 +1901,7 @@
         <v>2</v>
       </c>
       <c r="G65" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
@@ -1921,7 +1921,7 @@
         <v>2</v>
       </c>
       <c r="G66" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
@@ -1941,7 +1941,7 @@
         <v>2</v>
       </c>
       <c r="G67" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
@@ -1961,7 +1961,7 @@
         <v>2</v>
       </c>
       <c r="G68" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
@@ -1981,7 +1981,7 @@
         <v>2</v>
       </c>
       <c r="G69" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
@@ -2001,7 +2001,7 @@
         <v>2</v>
       </c>
       <c r="G70" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
@@ -2021,7 +2021,7 @@
         <v>2</v>
       </c>
       <c r="G71" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
@@ -2041,7 +2041,7 @@
         <v>2</v>
       </c>
       <c r="G72" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
@@ -2061,7 +2061,7 @@
         <v>2</v>
       </c>
       <c r="G73" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
@@ -2081,7 +2081,7 @@
         <v>1</v>
       </c>
       <c r="G74" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
@@ -2101,7 +2101,7 @@
         <v>1</v>
       </c>
       <c r="G75" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
@@ -2121,7 +2121,7 @@
         <v>1</v>
       </c>
       <c r="G76" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
@@ -2141,7 +2141,7 @@
         <v>1</v>
       </c>
       <c r="G77" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
@@ -2161,7 +2161,7 @@
         <v>1</v>
       </c>
       <c r="G78" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
@@ -2181,7 +2181,7 @@
         <v>1</v>
       </c>
       <c r="G79" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
@@ -2201,7 +2201,7 @@
         <v>1</v>
       </c>
       <c r="G80" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
@@ -2221,7 +2221,7 @@
         <v>1</v>
       </c>
       <c r="G81" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
@@ -2241,7 +2241,7 @@
         <v>1</v>
       </c>
       <c r="G82" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
@@ -2261,7 +2261,7 @@
         <v>1</v>
       </c>
       <c r="G83" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
@@ -2281,7 +2281,7 @@
         <v>1</v>
       </c>
       <c r="G84" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
@@ -2301,7 +2301,7 @@
         <v>1</v>
       </c>
       <c r="G85" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
@@ -2321,7 +2321,7 @@
         <v>1</v>
       </c>
       <c r="G86" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
@@ -2341,7 +2341,7 @@
         <v>2</v>
       </c>
       <c r="G87" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
@@ -2361,7 +2361,7 @@
         <v>2</v>
       </c>
       <c r="G88" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
@@ -2381,7 +2381,7 @@
         <v>2</v>
       </c>
       <c r="G89" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
@@ -2401,7 +2401,7 @@
         <v>2</v>
       </c>
       <c r="G90" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
@@ -2421,7 +2421,7 @@
         <v>2</v>
       </c>
       <c r="G91" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
@@ -2441,7 +2441,7 @@
         <v>2</v>
       </c>
       <c r="G92" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
@@ -2461,7 +2461,7 @@
         <v>2</v>
       </c>
       <c r="G93" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
@@ -2481,7 +2481,7 @@
         <v>1</v>
       </c>
       <c r="G94" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
@@ -2501,7 +2501,7 @@
         <v>1</v>
       </c>
       <c r="G95" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
@@ -2521,7 +2521,7 @@
         <v>1</v>
       </c>
       <c r="G96" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
@@ -2541,7 +2541,7 @@
         <v>1</v>
       </c>
       <c r="G97" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
@@ -2561,7 +2561,7 @@
         <v>1</v>
       </c>
       <c r="G98" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
@@ -2581,7 +2581,7 @@
         <v>1</v>
       </c>
       <c r="G99" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
@@ -2601,7 +2601,7 @@
         <v>1</v>
       </c>
       <c r="G100" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
@@ -2621,7 +2621,7 @@
         <v>1</v>
       </c>
       <c r="G101" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
@@ -2641,7 +2641,7 @@
         <v>1</v>
       </c>
       <c r="G102" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
@@ -2661,7 +2661,7 @@
         <v>1</v>
       </c>
       <c r="G103" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
@@ -2681,7 +2681,7 @@
         <v>1</v>
       </c>
       <c r="G104" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
@@ -2701,7 +2701,7 @@
         <v>1</v>
       </c>
       <c r="G105" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
@@ -2721,7 +2721,7 @@
         <v>1</v>
       </c>
       <c r="G106" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
@@ -2741,7 +2741,7 @@
         <v>1</v>
       </c>
       <c r="G107" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
@@ -2761,7 +2761,7 @@
         <v>1</v>
       </c>
       <c r="G108" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
@@ -2781,7 +2781,7 @@
         <v>1</v>
       </c>
       <c r="G109" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
@@ -2801,7 +2801,7 @@
         <v>1</v>
       </c>
       <c r="G110" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
@@ -2821,7 +2821,7 @@
         <v>1</v>
       </c>
       <c r="G111" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
@@ -2841,7 +2841,7 @@
         <v>1</v>
       </c>
       <c r="G112" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
@@ -2861,7 +2861,7 @@
         <v>1</v>
       </c>
       <c r="G113" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.2">
@@ -2881,7 +2881,7 @@
         <v>1</v>
       </c>
       <c r="G114" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
@@ -2901,7 +2901,7 @@
         <v>1</v>
       </c>
       <c r="G115" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
@@ -2921,7 +2921,7 @@
         <v>2</v>
       </c>
       <c r="G116" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
@@ -2941,7 +2941,7 @@
         <v>2</v>
       </c>
       <c r="G117" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
@@ -2961,7 +2961,7 @@
         <v>2</v>
       </c>
       <c r="G118" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
@@ -2981,7 +2981,7 @@
         <v>2</v>
       </c>
       <c r="G119" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.2">
@@ -3001,7 +3001,7 @@
         <v>2</v>
       </c>
       <c r="G120" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.2">
@@ -3021,7 +3021,7 @@
         <v>2</v>
       </c>
       <c r="G121" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.2">
@@ -3041,7 +3041,7 @@
         <v>2</v>
       </c>
       <c r="G122" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.2">
@@ -3061,7 +3061,7 @@
         <v>2</v>
       </c>
       <c r="G123" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.2">
@@ -3081,7 +3081,7 @@
         <v>2</v>
       </c>
       <c r="G124" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.2">
@@ -3101,7 +3101,7 @@
         <v>2</v>
       </c>
       <c r="G125" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>